<commit_message>
Compares GDP estimations by region
</commit_message>
<xml_diff>
--- a/PabloArriagada/maddison_database_project/data/Regional composition_web.xlsx
+++ b/PabloArriagada/maddison_database_project/data/Regional composition_web.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\Google Drive\OWID\notebooks\maddison_database_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A86C659-4501-47EF-BF3C-C7879B12D97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9750E422-E1C7-45F5-A7A1-70241B25A299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B7B0E0DB-4549-4FE2-A1CC-B49F57401426}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="146">
   <si>
     <t>Western Europe</t>
   </si>
@@ -5575,10 +5575,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BEAAA1A-DDC7-4492-8D62-63F8428A4F84}">
-  <dimension ref="A1:C305"/>
+  <dimension ref="A1:C301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
+      <selection activeCell="C305" sqref="A302:C305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8894,50 +8894,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A302" t="s">
-        <v>10</v>
-      </c>
-      <c r="B302">
-        <v>1950</v>
-      </c>
-      <c r="C302" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A303" t="s">
-        <v>24</v>
-      </c>
-      <c r="B303">
-        <v>1950</v>
-      </c>
-      <c r="C303" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A304" t="s">
-        <v>38</v>
-      </c>
-      <c r="B304">
-        <v>1950</v>
-      </c>
-      <c r="C304" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A305" t="s">
-        <v>48</v>
-      </c>
-      <c r="B305">
-        <v>1950</v>
-      </c>
-      <c r="C305" t="s">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1:C305" xr:uid="{5BEAAA1A-DDC7-4492-8D62-63F8428A4F84}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>